<commit_message>
Upload Chapter 18 - Female Genital Cutting
</commit_message>
<xml_diff>
--- a/DHS7tabplan/Tab_Plan_Chap09_Reproductive_Health_VII_5Sept2018.xlsx
+++ b/DHS7tabplan/Tab_Plan_Chap09_Reproductive_Health_VII_5Sept2018.xlsx
@@ -10438,8 +10438,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3299ADD5D91FC4981A62029954D61DA" ma:contentTypeVersion="476" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95dfcc87ed256f4aed73fd9ca228c514">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd" xmlns:ns3="d16efad5-0601-4cf0-b7c2-89968258c777" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88209df52733b038c0f2ab805b0d468e" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3299ADD5D91FC4981A62029954D61DA" ma:contentTypeVersion="533" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9fe6dd6fbc47b2b2c3033f1a9c1079fd">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd" xmlns:ns3="d16efad5-0601-4cf0-b7c2-89968258c777" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fd9e5a0c56088652e9b5d1a36fcd7f8a" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd"/>
     <xsd:import namespace="d16efad5-0601-4cf0-b7c2-89968258c777"/>
@@ -10463,6 +10463,10 @@
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:Survey_x0020_Type" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -10525,6 +10529,28 @@
           <xsd:enumeration value="DHS"/>
           <xsd:enumeration value="MIS"/>
           <xsd:enumeration value="SPA"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="23" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="24" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="25" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="26" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
@@ -10742,10 +10768,10 @@
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
-    <_dlc_DocId xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">VMX3MACP777Z-432858100-6934</_dlc_DocId>
+    <_dlc_DocId xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">VMX3MACP777Z-432858100-14094</_dlc_DocId>
     <_dlc_DocIdUrl xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">
-      <Url>https://icfonline.sharepoint.com/sites/ihd-dhs/Analysis/_layouts/15/DocIdRedir.aspx?ID=VMX3MACP777Z-432858100-6934</Url>
-      <Description>VMX3MACP777Z-432858100-6934</Description>
+      <Url>https://icfonline.sharepoint.com/sites/ihd-dhs/Analysis/_layouts/15/DocIdRedir.aspx?ID=VMX3MACP777Z-432858100-14094</Url>
+      <Description>VMX3MACP777Z-432858100-14094</Description>
     </_dlc_DocIdUrl>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <Survey_x0020_Type xmlns="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd">DHS</Survey_x0020_Type>
@@ -10755,7 +10781,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AED6AB5-416D-40FA-ABF5-11F6C9DB4583}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DBEA9AF-996C-4E7C-B553-9A1F1EC22837}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>